<commit_message>
adding same hvg option
</commit_message>
<xml_diff>
--- a/gepdynamics/static/fingerprint_template.xlsx
+++ b/gepdynamics/static/fingerprint_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yotamcon/projects/gep-dynamics/gepdynamics/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0EFD52-0B13-E246-9806-6079D8DA4874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785920D1-594C-CA43-A596-F62CE5BBD1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1900" windowWidth="21620" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10320" yWindow="1560" windowWidth="21620" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tst" sheetId="1" r:id="rId1"/>
@@ -969,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I126" sqref="I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1618,6 +1618,1086 @@
       <c r="G62" s="4"/>
       <c r="H62" s="5"/>
     </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="4"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="4"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="4"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="4"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="4"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="4"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="4"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="5"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="4"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="4"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="4"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="4"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="4"/>
+      <c r="H104" s="5"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="4"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="5"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="4"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="5"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="4"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="5"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="4"/>
+      <c r="B111" s="5"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="5"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="5"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="4"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="5"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="4"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="4"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="4"/>
+      <c r="H116" s="5"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="4"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="5"/>
+      <c r="G117" s="4"/>
+      <c r="H117" s="5"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="4"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="5"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="5"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="3"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="5"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="4"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="5"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="4"/>
+      <c r="B123" s="5"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="5"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="4"/>
+      <c r="B124" s="5"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="5"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="4"/>
+      <c r="B125" s="5"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="5"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="5"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" s="4"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="5"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="5"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="4"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="5"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="5"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="B131" s="5"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="5"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="4"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="5"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+      <c r="H135" s="5"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" s="4"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="5"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="5"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="5"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="5"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="4"/>
+      <c r="F138" s="5"/>
+      <c r="G138" s="4"/>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="4"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="4"/>
+      <c r="H139" s="5"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="3"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+      <c r="C142" s="4"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="5"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" s="4"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="5"/>
+      <c r="G143" s="4"/>
+      <c r="H143" s="5"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" s="4"/>
+      <c r="B144" s="5"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="5"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="5"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" s="4"/>
+      <c r="B145" s="5"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="5"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="4"/>
+      <c r="B146" s="5"/>
+      <c r="C146" s="4"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="4"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="4"/>
+      <c r="H146" s="5"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="3"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="C149" s="4"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="4"/>
+      <c r="F149" s="4"/>
+      <c r="G149" s="4"/>
+      <c r="H149" s="5"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="4"/>
+      <c r="B150" s="5"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="4"/>
+      <c r="H150" s="5"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="4"/>
+      <c r="B151" s="5"/>
+      <c r="C151" s="4"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="5"/>
+      <c r="G151" s="4"/>
+      <c r="H151" s="5"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="4"/>
+      <c r="B152" s="5"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="5"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="5"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="4"/>
+      <c r="B153" s="5"/>
+      <c r="C153" s="4"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="4"/>
+      <c r="F153" s="5"/>
+      <c r="G153" s="4"/>
+      <c r="H153" s="5"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
+      <c r="H155" s="3"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+      <c r="H156" s="5"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" s="4"/>
+      <c r="B157" s="5"/>
+      <c r="C157" s="4"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="4"/>
+      <c r="F157" s="5"/>
+      <c r="G157" s="4"/>
+      <c r="H157" s="5"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" s="4"/>
+      <c r="B158" s="5"/>
+      <c r="C158" s="4"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="4"/>
+      <c r="F158" s="5"/>
+      <c r="G158" s="4"/>
+      <c r="H158" s="5"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" s="4"/>
+      <c r="B159" s="5"/>
+      <c r="C159" s="4"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="4"/>
+      <c r="F159" s="5"/>
+      <c r="G159" s="4"/>
+      <c r="H159" s="5"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" s="4"/>
+      <c r="B160" s="5"/>
+      <c r="C160" s="4"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="4"/>
+      <c r="F160" s="5"/>
+      <c r="G160" s="4"/>
+      <c r="H160" s="5"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" s="3"/>
+      <c r="B162" s="3"/>
+      <c r="C162" s="3"/>
+      <c r="D162" s="3"/>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3"/>
+      <c r="H162" s="3"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+      <c r="H163" s="5"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" s="4"/>
+      <c r="B164" s="5"/>
+      <c r="C164" s="4"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="4"/>
+      <c r="F164" s="5"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="5"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" s="4"/>
+      <c r="B165" s="5"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="5"/>
+      <c r="G165" s="4"/>
+      <c r="H165" s="5"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" s="4"/>
+      <c r="B166" s="5"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="5"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="5"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" s="4"/>
+      <c r="B167" s="5"/>
+      <c r="C167" s="4"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="4"/>
+      <c r="F167" s="5"/>
+      <c r="G167" s="4"/>
+      <c r="H167" s="5"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" s="3"/>
+      <c r="B169" s="3"/>
+      <c r="C169" s="3"/>
+      <c r="D169" s="3"/>
+      <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+      <c r="G169" s="3"/>
+      <c r="H169" s="3"/>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" s="4"/>
+      <c r="B170" s="4"/>
+      <c r="C170" s="4"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="4"/>
+      <c r="F170" s="4"/>
+      <c r="G170" s="4"/>
+      <c r="H170" s="5"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" s="4"/>
+      <c r="B171" s="5"/>
+      <c r="C171" s="4"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="5"/>
+      <c r="G171" s="4"/>
+      <c r="H171" s="5"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" s="4"/>
+      <c r="B172" s="5"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="4"/>
+      <c r="F172" s="5"/>
+      <c r="G172" s="4"/>
+      <c r="H172" s="5"/>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" s="4"/>
+      <c r="B173" s="5"/>
+      <c r="C173" s="4"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="4"/>
+      <c r="F173" s="5"/>
+      <c r="G173" s="4"/>
+      <c r="H173" s="5"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" s="4"/>
+      <c r="B174" s="5"/>
+      <c r="C174" s="4"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="5"/>
+      <c r="G174" s="4"/>
+      <c r="H174" s="5"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" s="3"/>
+      <c r="B176" s="3"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="3"/>
+      <c r="E176" s="3"/>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
+      <c r="H176" s="3"/>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="5"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" s="4"/>
+      <c r="B178" s="5"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="5"/>
+      <c r="G178" s="4"/>
+      <c r="H178" s="5"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" s="4"/>
+      <c r="B179" s="5"/>
+      <c r="C179" s="4"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="5"/>
+      <c r="G179" s="4"/>
+      <c r="H179" s="5"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" s="4"/>
+      <c r="B180" s="5"/>
+      <c r="C180" s="4"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="5"/>
+      <c r="G180" s="4"/>
+      <c r="H180" s="5"/>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" s="4"/>
+      <c r="B181" s="5"/>
+      <c r="C181" s="4"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="5"/>
+      <c r="G181" s="4"/>
+      <c r="H181" s="5"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183" s="3"/>
+      <c r="B183" s="3"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="3"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="3"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184" s="4"/>
+      <c r="B184" s="4"/>
+      <c r="C184" s="4"/>
+      <c r="D184" s="5"/>
+      <c r="E184" s="4"/>
+      <c r="F184" s="4"/>
+      <c r="G184" s="4"/>
+      <c r="H184" s="5"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185" s="4"/>
+      <c r="B185" s="5"/>
+      <c r="C185" s="4"/>
+      <c r="D185" s="5"/>
+      <c r="E185" s="4"/>
+      <c r="F185" s="5"/>
+      <c r="G185" s="4"/>
+      <c r="H185" s="5"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" s="4"/>
+      <c r="B186" s="5"/>
+      <c r="C186" s="4"/>
+      <c r="D186" s="5"/>
+      <c r="E186" s="4"/>
+      <c r="F186" s="5"/>
+      <c r="G186" s="4"/>
+      <c r="H186" s="5"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187" s="4"/>
+      <c r="B187" s="5"/>
+      <c r="C187" s="4"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="4"/>
+      <c r="F187" s="5"/>
+      <c r="G187" s="4"/>
+      <c r="H187" s="5"/>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" s="4"/>
+      <c r="B188" s="5"/>
+      <c r="C188" s="4"/>
+      <c r="D188" s="5"/>
+      <c r="E188" s="4"/>
+      <c r="F188" s="5"/>
+      <c r="G188" s="4"/>
+      <c r="H188" s="5"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576 D1:D1048576 F1:F1048576 H1:H1048576">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Altering fingerprint template view position
</commit_message>
<xml_diff>
--- a/gepdynamics/static/fingerprint_template.xlsx
+++ b/gepdynamics/static/fingerprint_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yotamcon/projects/gep-dynamics/gepdynamics/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785920D1-594C-CA43-A596-F62CE5BBD1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1767AC19-5AFF-1146-891B-8321849426C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10320" yWindow="1560" windowWidth="21620" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -971,9 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I126" sqref="I126"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>